<commit_message>
Consolidado das estimativas de posição com 4 nos
0,50 metros
1 metros
2 metros
</commit_message>
<xml_diff>
--- a/Save_Data_experimento_v3/Save_Data/estimativa de posicao com 4 nos/estimativa_posicao_4nos.xlsx
+++ b/Save_Data_experimento_v3/Save_Data/estimativa de posicao com 4 nos/estimativa_posicao_4nos.xlsx
@@ -5,20 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\UTFPR\2021.1\TCC1\Codigos\Save_Data_experimento_v2\Save_Data\estimativa de posicao com 4 nos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\UTFPR\2021.1\TCC1\Codigos\Save_Data_experimento_v3\Save_Data\estimativa de posicao com 4 nos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3E3691-E144-4E8D-83D4-B6A9D0752B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D925A8-3A93-4235-A02C-BDAD04CF20C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1632" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23664" yWindow="624" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -420,12 +428,12 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -463,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -501,7 +509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -539,7 +547,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -577,7 +585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -615,7 +623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>

</xml_diff>